<commit_message>
Normalement la version final
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\РА\Documents\programme\python\PFE-V3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Identification" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="228">
   <si>
     <t>Sexe</t>
   </si>
@@ -692,6 +697,21 @@
   </si>
   <si>
     <t>Laboratoire d'affiliation du co- Directeur de thèse</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>pdp\C16026ERER.jpg</t>
+  </si>
+  <si>
+    <t>pdp\C18023TECI.png</t>
+  </si>
+  <si>
+    <t>pdp\C18026TECI.png</t>
+  </si>
+  <si>
+    <t>pdp\C18005ELSY.png</t>
   </si>
 </sst>
 </file>
@@ -777,7 +797,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -786,12 +806,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -833,7 +856,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,7 +891,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1077,29 +1100,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="26.77734375" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="24.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>210</v>
       </c>
@@ -1136,8 +1159,11 @@
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1174,8 +1200,11 @@
       <c r="L2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1212,8 +1241,11 @@
       <c r="L3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1250,8 +1282,11 @@
       <c r="L4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1279,23 +1314,26 @@
       <c r="I5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G9" s="3"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="3"/>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G28" s="3"/>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G31" s="3"/>
     </row>
-    <row r="48" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G48" s="3"/>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G50" s="3"/>
     </row>
   </sheetData>
@@ -1312,18 +1350,18 @@
       <selection activeCell="A6" sqref="A6:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="49.88671875" customWidth="1"/>
-    <col min="5" max="5" width="62.6640625" customWidth="1"/>
-    <col min="7" max="7" width="62.5546875" customWidth="1"/>
-    <col min="8" max="8" width="31.109375" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="62.7109375" customWidth="1"/>
+    <col min="7" max="7" width="62.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1352,7 +1390,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1381,7 +1419,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1410,7 +1448,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1436,7 +1474,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1475,19 +1513,19 @@
       <selection activeCell="A6" sqref="A6:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" customWidth="1"/>
-    <col min="6" max="6" width="33.21875" customWidth="1"/>
-    <col min="7" max="8" width="42.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="7" max="8" width="42.7109375" customWidth="1"/>
     <col min="9" max="9" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -1513,7 +1551,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1539,7 +1577,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>75</v>
       </c>
@@ -1553,7 +1591,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -1567,7 +1605,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1594,12 +1632,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>219</v>
       </c>
@@ -1607,7 +1645,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1615,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2016</v>
       </c>
@@ -1623,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -1631,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2018</v>
       </c>
@@ -1652,16 +1690,16 @@
       <selection activeCell="A6" sqref="A6:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="61.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="61.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>93</v>
       </c>
@@ -1678,7 +1716,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1695,7 +1733,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -1712,7 +1750,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -1729,7 +1767,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -1746,58 +1784,58 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
     </row>
   </sheetData>
@@ -1813,22 +1851,22 @@
       <selection activeCell="A6" sqref="A6:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="46.88671875" customWidth="1"/>
-    <col min="4" max="4" width="48.109375" customWidth="1"/>
-    <col min="5" max="5" width="35.21875" customWidth="1"/>
-    <col min="6" max="6" width="37.109375" customWidth="1"/>
-    <col min="7" max="7" width="26.77734375" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
-    <col min="9" max="9" width="32.33203125" customWidth="1"/>
-    <col min="10" max="10" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32.28515625" customWidth="1"/>
+    <col min="10" max="10" width="32.42578125" customWidth="1"/>
     <col min="11" max="11" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -1863,7 +1901,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1898,7 +1936,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>120</v>
       </c>
@@ -1927,7 +1965,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1953,7 +1991,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1988,51 +2026,51 @@
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H6" s="3"/>
       <c r="J6" s="2"/>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K8" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G10" s="2"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K18" s="3"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2067,7 +2105,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>125</v>
       </c>
@@ -2099,7 +2137,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>126</v>
       </c>
@@ -2128,7 +2166,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>127</v>
       </c>
@@ -2160,7 +2198,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2225,19 +2263,19 @@
       <selection activeCell="A6" sqref="A6:XFD98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.5546875" customWidth="1"/>
-    <col min="2" max="2" width="39.109375" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.44140625" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" customWidth="1"/>
-    <col min="8" max="8" width="65.77734375" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="65.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2267,7 +2305,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -2293,7 +2331,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>188</v>
       </c>
@@ -2316,7 +2354,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>189</v>
       </c>
@@ -2339,7 +2377,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>190</v>
       </c>
@@ -2362,196 +2400,196 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H17" s="3"/>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H20" s="3"/>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H27" s="3"/>
     </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H33" s="3"/>
     </row>
-    <row r="35" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H36" s="3"/>
     </row>
-    <row r="38" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G60" s="3"/>
     </row>
-    <row r="62" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H64" s="3"/>
     </row>
-    <row r="65" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H65" s="3"/>
     </row>
-    <row r="66" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G66" s="2"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G67" s="2"/>
       <c r="H67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="72" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H72" s="3"/>
     </row>
-    <row r="73" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H73" s="3"/>
     </row>
-    <row r="74" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H74" s="3"/>
     </row>
-    <row r="75" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:12" x14ac:dyDescent="0.25">
       <c r="H75" s="3"/>
     </row>
-    <row r="76" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G76" s="3"/>
     </row>
-    <row r="78" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G78" s="3"/>
     </row>
-    <row r="80" spans="7:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G80" s="3"/>
     </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" s="3"/>
     </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G82" s="3"/>
     </row>
   </sheetData>
@@ -2573,18 +2611,18 @@
       <selection activeCell="A6" sqref="A6:XFD22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="4" width="36.88671875" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" customWidth="1"/>
-    <col min="7" max="7" width="40.109375" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>183</v>
       </c>
@@ -2608,7 +2646,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2631,7 +2669,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>120</v>
       </c>
@@ -2651,12 +2689,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2676,37 +2714,37 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G16" s="3"/>
     </row>
   </sheetData>

</xml_diff>